<commit_message>
Modified dummy values and property names
</commit_message>
<xml_diff>
--- a/Ontology/Factory/buildingScenario.xlsx
+++ b/Ontology/Factory/buildingScenario.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GAURAV SRIVASTAVA\Desktop\TCS Internship\Task 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GAURAV SRIVASTAVA\Documents\GitHub\DigitalTwin\Ontology\Factory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF44381E-67E5-40BC-A827-90B9A8500C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF66746C-2646-45EA-9DA1-600A75304895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{B6154E4F-774F-4730-84F3-5195ADBCD94E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>ModelID</t>
   </si>
@@ -45,58 +45,257 @@
     <t>contains</t>
   </si>
   <si>
-    <t>FacFloor1</t>
-  </si>
-  <si>
-    <t>FacFloor0</t>
-  </si>
-  <si>
-    <t>RoboP1</t>
-  </si>
-  <si>
-    <t>RoboP2</t>
-  </si>
-  <si>
-    <t>RoboP3</t>
-  </si>
-  <si>
-    <t>RoboP4</t>
-  </si>
-  <si>
-    <t>RoboP5</t>
-  </si>
-  <si>
-    <t>RoboP6</t>
-  </si>
-  <si>
-    <t>RoboP7</t>
-  </si>
-  <si>
-    <t>RoboP8</t>
-  </si>
-  <si>
-    <t>RoboP9</t>
-  </si>
-  <si>
-    <t>DTBuildingA</t>
-  </si>
-  <si>
-    <t>dtmi:Digital_Twin_Proj:DTBuilding;1</t>
-  </si>
-  <si>
-    <t>dtmi:Digital_Twin_Proj:FacFloor;1</t>
-  </si>
-  <si>
-    <t>dtmi:Digital_Twin_Proj:RoboP;1</t>
-  </si>
-  <si>
-    <t>{}</t>
-  </si>
-  <si>
-    <t>{5,0.16,"Working",5000,"RoboP10"</t>
-  </si>
-  <si>
-    <t>RoboP10</t>
+    <t>FactoryFloor0</t>
+  </si>
+  <si>
+    <t>FactoryFloor1</t>
+  </si>
+  <si>
+    <t>RoboticPalletizer1</t>
+  </si>
+  <si>
+    <t>RoboticPalletizer2</t>
+  </si>
+  <si>
+    <t>RoboticPalletizer3</t>
+  </si>
+  <si>
+    <t>RoboticPalletizer4</t>
+  </si>
+  <si>
+    <t>RoboticPalletizer5</t>
+  </si>
+  <si>
+    <t>RoboticPalletizer6</t>
+  </si>
+  <si>
+    <t>RoboticPalletizer7</t>
+  </si>
+  <si>
+    <t>RoboticPalletizer8</t>
+  </si>
+  <si>
+    <t>RoboticPalletizer9</t>
+  </si>
+  <si>
+    <t>RoboticPalletizer10</t>
+  </si>
+  <si>
+    <t>BuildingA</t>
+  </si>
+  <si>
+    <t>dtmi:DigitalTwin:Building;1</t>
+  </si>
+  <si>
+    <t>dtmi:DigitalTwin:FactoryFloor;1</t>
+  </si>
+  <si>
+    <t>dtmi:DigitalTwin:RoboticPalletizer;1</t>
+  </si>
+  <si>
+    <t>{
+   "Temperature": 25,
+   "Humidity": 60,
+   "Area": 20000,
+   "NumberofRobotPalletizers": 5
+}</t>
+  </si>
+  <si>
+    <t>{
+   "Temperature": 27,
+   "Humidity": 63,
+   "Area": 20000,
+   "NumberofRobotPalletizers": 5
+}</t>
+  </si>
+  <si>
+    <t>{
+   "Address": {
+      "Street": "21, Okhla Industrial Area",
+      "City": "Delhi",
+      "State": "Delhi",
+      "Country": "India",
+      "Zip": "110001"
+   },
+   "GeographicalCoordinates": {
+      "Latitude": 28.6139,
+      "Longitude": 77.2090
+   },
+   "Altitude": 50,
+   "SiteArea": 20000,
+   "Numberoffloors": 2,
+   "EnergyConsumption": 75000
+}</t>
+  </si>
+  <si>
+    <t>{
+   "RoboticArmID":"RA-12345",
+   "Status":"Active",
+   "RoboticArmPowerConsumption":500,
+   "RoboticArmOperatingSpeed":60,
+   "RoboticArmLoadCapacity":1000,
+   "ConveyorBeltSpeed":0.5,
+   "LightCurtainResolution":0.01,
+   "LightCurtainRange":10,
+   "PalletArea":25,
+   "LastAccessedTime":"2023-09-22 14:30:00",
+   "PlasticWrappingSpeed":30,
+   "FilmRollStatus":"OK",
+   "WrappingFilmUsage":150
+}</t>
+  </si>
+  <si>
+    <t>{
+"RoboticArmID":"RA-67890",
+"Status":"Inactive",
+"RoboticArmPowerConsumption":750,
+"RoboticArmOperatingSpeed":45,
+"RoboticArmLoadCapacity":1200,
+"ConveyorBeltSpeed":0.6,
+"LightCurtainResolution":0.015,
+"LightCurtainRange":12,
+"PalletArea":30,
+"LastAccessedTime":"2023-09-22 15:45:00",
+"PlasticWrappingSpeed":25,
+"FilmRollStatus":"Low",
+"WrappingFilmUsage":200
+}</t>
+  </si>
+  <si>
+    <t>{
+"RoboticArmID":"RA-54321",
+"Status":"Active",
+"RoboticArmPowerConsumption":600,
+"RoboticArmOperatingSpeed":55,
+"RoboticArmLoadCapacity":900,
+"ConveyorBeltSpeed":0.7,
+"LightCurtainResolution":0.02,
+"LightCurtainRange":8,
+"PalletArea":20,
+"LastAccessedTime":"2023-09-22 16:15:00",
+"PlasticWrappingSpeed":35,
+"FilmRollStatus":"OK",
+"WrappingFilmUsage":100
+}</t>
+  </si>
+  <si>
+    <t>{
+"RoboticArmID":"RA-98765",
+"Status":"Active",
+"RoboticArmPowerConsumption":800,
+"RoboticArmOperatingSpeed":70,
+"RoboticArmLoadCapacity":1500,
+"ConveyorBeltSpeed":0.8,
+"LightCurtainResolution":0.025,
+"LightCurtainRange":15,
+"PalletArea":35,
+"LastAccessedTime":"2023-09-22 17:00:00",
+"PlasticWrappingSpeed":40,
+"FilmRollStatus":"OK",
+"WrappingFilmUsage":180
+}</t>
+  </si>
+  <si>
+    <t>{
+"RoboticArmID":"RA-23456",
+"Status":"Inactive",
+"RoboticArmPowerConsumption":700,
+"RoboticArmOperatingSpeed":50,
+"RoboticArmLoadCapacity":1100,
+"ConveyorBeltSpeed":0.5,
+"LightCurtainResolution":0.012,
+"LightCurtainRange":11,
+"PalletArea":27,
+"LastAccessedTime":"2023-09-22 18:30:00",
+"PlasticWrappingSpeed":28,
+"FilmRollStatus":"Low",
+"WrappingFilmUsage":220
+}</t>
+  </si>
+  <si>
+    <t>{
+"RoboticArmID":"RA-76543",
+"Status":"Active",
+"RoboticArmPowerConsumption":550,
+"RoboticArmOperatingSpeed":65,
+"RoboticArmLoadCapacity":800,
+"ConveyorBeltSpeed":0.9,
+"LightCurtainResolution":0.018,
+"LightCurtainRange":14,
+"PalletArea":32,
+"LastAccessedTime":"2023-09-22 19:45:00",
+"PlasticWrappingSpeed":33,
+"FilmRollStatus":"OK",
+"WrappingFilmUsage":120
+}</t>
+  </si>
+  <si>
+    <t>{
+"RoboticArmID":"RA-34567",
+"Status":"Active",
+"RoboticArmPowerConsumption":650,
+"RoboticArmOperatingSpeed":58,
+"RoboticArmLoadCapacity":1000,
+"ConveyorBeltSpeed":0.6,
+"LightCurtainResolution":0.016,
+"LightCurtainRange":13,
+"PalletArea":29,
+"LastAccessedTime":"2023-09-22 20:15:00",
+"PlasticWrappingSpeed":36,
+"FilmRollStatus":"OK",
+"WrappingFilmUsage":160
+}</t>
+  </si>
+  <si>
+    <t>{
+"RoboticArmID":"RA-87654",
+"Status":"Inactive",
+"RoboticArmPowerConsumption":750,
+"RoboticArmOperatingSpeed":48,
+"RoboticArmLoadCapacity":1300,
+"ConveyorBeltSpeed":0.7,
+"LightCurtainResolution":0.021,
+"LightCurtainRange":9,
+"PalletArea":22,
+"LastAccessedTime":"2023-09-22 21:30:00",
+"PlasticWrappingSpeed":31,
+"FilmRollStatus":"Low",
+"WrappingFilmUsage":190
+}</t>
+  </si>
+  <si>
+    <t>{
+"RoboticArmID":"RA-45678",
+"Status":"Active",
+"RoboticArmPowerConsumption":600,
+"RoboticArmOperatingSpeed":55,
+"RoboticArmLoadCapacity":950,
+"ConveyorBeltSpeed":0.8,
+"LightCurtainResolution":0.022,
+"LightCurtainRange":10,
+"PalletArea":24,
+"LastAccessedTime":"2023-09-22 22:00:00",
+"PlasticWrappingSpeed":34,
+"FilmRollStatus":"OK",
+"WrappingFilmUsage":140
+}</t>
+  </si>
+  <si>
+    <t>{
+"RoboticArmID":"RA-54321",
+"Status":"Inactive",
+"RoboticArmPowerConsumption":700,
+"RoboticArmOperatingSpeed":52,
+"RoboticArmLoadCapacity":1050,
+"ConveyorBeltSpeed":0.5,
+"LightCurtainResolution":0.019,
+"LightCurtainRange":12,
+"PalletArea":28,
+"LastAccessedTime":"2023-09-22 23:30:00",
+"PlasticWrappingSpeed":29,
+"FilmRollStatus":"Low",
+"WrappingFilmUsage":210
+}</t>
   </si>
 </sst>
 </file>
@@ -138,8 +337,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E4B3A2-EF53-41B2-9F0F-6F5502ACE162}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,186 +688,219 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
-      <c r="E14" t="s">
-        <v>22</v>
+      <c r="E14" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>